<commit_message>
combined two data sheets into one
</commit_message>
<xml_diff>
--- a/data/yummy_recipes.xlsx
+++ b/data/yummy_recipes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\meal-plan\meal-plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA459221-052D-4578-8C93-EACEA376F964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F94C61-CD32-47DA-85B1-7AD04C0F088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="recipes" sheetId="1" r:id="rId1"/>
+    <sheet name="additional" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>https://www.allrecipes.com/recipe/158968/spinach-and-feta-turkey-burgers/</t>
   </si>
@@ -34,6 +35,33 @@
   </si>
   <si>
     <t>urls</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>1 bag of Barbeque Chips</t>
+  </si>
+  <si>
+    <t>1 loaf of sliced bread</t>
+  </si>
+  <si>
+    <t>1 package of colby jack cheese</t>
+  </si>
+  <si>
+    <t>1 package of sliced turkey</t>
+  </si>
+  <si>
+    <t>paper towels</t>
+  </si>
+  <si>
+    <t>non-ingredient</t>
+  </si>
+  <si>
+    <t>toilet paper</t>
   </si>
 </sst>
 </file>
@@ -365,26 +393,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="72.5703125" customWidth="1"/>
+    <col min="1" max="1" width="72.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -397,4 +425,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63316E3-DAF7-448C-A1AD-F7E443C3762C}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="55.83984375" customWidth="1"/>
+    <col min="2" max="2" width="19.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made it so it doesn't pick random recipes
</commit_message>
<xml_diff>
--- a/data/yummy_recipes.xlsx
+++ b/data/yummy_recipes.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\meal-plan\meal-plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933842FC-D29C-4846-BF56-7465C02745AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1019701E-2A9A-4BCA-BDF4-7E1D21201F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recipes" sheetId="1" r:id="rId1"/>
     <sheet name="additional" sheetId="2" r:id="rId2"/>
     <sheet name="all_additional_items" sheetId="3" r:id="rId3"/>
+    <sheet name="all_recipes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>urls</t>
   </si>
@@ -159,6 +160,9 @@
   </si>
   <si>
     <t>https://www.allrecipes.com/recipe/228823/quick-beef-stir-fry/</t>
+  </si>
+  <si>
+    <t>anything premade</t>
   </si>
 </sst>
 </file>
@@ -498,78 +502,57 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.578125" customWidth="1"/>
+    <col min="1" max="1" width="72.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{71C9C92E-BCB9-48B7-8EA1-01F04EC14AA2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{041221A0-58DC-46C0-AE5C-0FDBB4B2D85B}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{87A068A2-7D1F-40C1-A42C-6BD1F63A02FC}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{B51DFFE0-ECEE-4DB7-ADC0-33533948F5D1}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{D92C971C-5BB3-47F3-8B5E-578160F9A731}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{23EAD6D1-3091-4AE4-AC20-26589C907067}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{7BA0013B-003C-4794-AA79-A5CFD1D497AD}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{BAA8351E-A85B-49ED-92D1-343D076DC86B}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{C0BCD335-A9A2-4D9D-9F79-C2DAF870EAAA}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C1454F69-D1CC-4072-A6BE-AB62B01D9B83}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4423AB93-097B-4000-A31D-C2E47745CAF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -578,16 +561,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.83984375" customWidth="1"/>
-    <col min="2" max="2" width="19.578125" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -595,57 +578,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -657,19 +640,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9BC077-CABC-40DD-9533-1D01791B0D65}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.578125" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -677,67 +660,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -745,7 +728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -753,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -761,32 +744,116 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B8EF32-80F5-49A5-A8DC-8A724AD1D299}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{DB8AB2BC-CAB3-472B-AC21-81AE0566E929}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5A85E07B-3E1B-46C7-90A1-45DE7DF1B91F}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{5CA7BF6E-2412-4F47-9262-4D1C2BC857CF}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{BE182DBC-4FAA-4919-ACC8-0F6E7EA04C75}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{A9660B68-FA88-484F-B63C-97575AA0FB82}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{DD34B27F-D82F-4762-A3DC-74D321BC218A}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{3F6FB65E-E6AE-4392-B921-06F9246D526A}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{FF10F176-2549-418C-905B-99198573DA88}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{542583A7-6449-4C0A-9F46-33A01943E5CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>